<commit_message>
Mostrar nombre de la persona logeada en todo el sistema
</commit_message>
<xml_diff>
--- a/SICE/PENDIENTES SICE.xlsx
+++ b/SICE/PENDIENTES SICE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\SICE\SICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9913BF21-D9FC-40E5-BCED-0CBD3F86535D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F9048E-1DE4-4956-BE9D-D5291AB2B0E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CDAD816-6EEF-4AF1-8E51-6EA1C6BD8C20}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Hacer que en las tablas no se pueda seleccionar más de una fila, como esta en las tablas de mantenimiento de estudiantes y de profesores.</t>
   </si>
@@ -55,13 +55,19 @@
   </si>
   <si>
     <t>CHECK✔</t>
+  </si>
+  <si>
+    <t>Entrar a mostrar estudiante y despues entrar a mostrar profesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ✔</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +101,12 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,11 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -165,6 +174,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,189 +500,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39C322C-DA7F-4708-AFAF-345848D0A1FE}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B6" sqref="B6:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="7" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="6"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Agregar Usuario con Nombre, Tablas sin editar, roles con Usuario y Nombre
</commit_message>
<xml_diff>
--- a/SICE/PENDIENTES SICE.xlsx
+++ b/SICE/PENDIENTES SICE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\SICE\SICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F9048E-1DE4-4956-BE9D-D5291AB2B0E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC9A6E-BB07-4CF5-B152-969D4297E423}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CDAD816-6EEF-4AF1-8E51-6EA1C6BD8C20}"/>
   </bookViews>
@@ -57,17 +57,17 @@
     <t>CHECK✔</t>
   </si>
   <si>
-    <t>Entrar a mostrar estudiante y despues entrar a mostrar profesor</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ✔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      ✔</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +107,13 @@
     </font>
     <font>
       <sz val="22"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -172,9 +179,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -186,6 +190,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +511,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:O6"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,161 +560,161 @@
       <c r="O2" s="3"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="7"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="14" t="s">
-        <v>9</v>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="13"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>